<commit_message>
initial contribution of CDM profiles to Alvearie
Signed-off-by: eggebraa <tegge@us.ibm.com>
</commit_message>
<xml_diff>
--- a/docs/0.1.0/StructureDefinition-attributed-provider-with-period.xlsx
+++ b/docs/0.1.0/StructureDefinition-attributed-provider-with-period.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="103">
   <si>
     <t>Path</t>
   </si>
@@ -206,7 +206,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>http://alvearie.io/fhir/StructureDefinition/attributed-provider-with-period</t>
+    <t>http://ibm.com/fhir/cdm/StructureDefinition/attributed-provider-with-period</t>
   </si>
   <si>
     <t>N/A</t>
@@ -215,7 +215,7 @@
     <t>Extension.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://alvearie.io/fhir/StructureDefinition/reference-with-period}
+    <t xml:space="preserve">Reference {http://ibm.com/fhir/cdm/StructureDefinition/reference-with-period}
 </t>
   </si>
   <si>
@@ -244,14 +244,11 @@
     <t>referencePeriod</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://alvearie.io/fhir/StructureDefinition/reference-period}
+    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/reference-period}
 </t>
   </si>
   <si>
-    <t>Optional Extensions Element</t>
-  </si>
-  <si>
-    <t>Optional Extension Element - found in all resources.</t>
+    <t>A time period in which the reference is valid</t>
   </si>
   <si>
     <t>Extension.value[x].reference</t>
@@ -1384,7 +1381,7 @@
         <v>74</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1455,7 +1452,7 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -1475,19 +1472,19 @@
         <v>37</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J10" t="s" s="2">
         <v>45</v>
       </c>
       <c r="K10" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="L10" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="L10" t="s" s="2">
+      <c r="M10" t="s" s="2">
         <v>79</v>
-      </c>
-      <c r="M10" t="s" s="2">
-        <v>80</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
@@ -1537,16 +1534,16 @@
         <v>37</v>
       </c>
       <c r="AE10" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF10" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG10" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH10" t="s" s="2">
         <v>81</v>
-      </c>
-      <c r="AF10" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG10" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH10" t="s" s="2">
-        <v>82</v>
       </c>
       <c r="AI10" t="s" s="2">
         <v>68</v>
@@ -1557,7 +1554,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -1577,19 +1574,19 @@
         <v>37</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J11" t="s" s="2">
         <v>57</v>
       </c>
       <c r="K11" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="L11" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="L11" t="s" s="2">
+      <c r="M11" t="s" s="2">
         <v>85</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>86</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
@@ -1600,46 +1597,46 @@
         <v>37</v>
       </c>
       <c r="R11" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="S11" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T11" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U11" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V11" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W11" t="s" s="2">
         <v>87</v>
       </c>
-      <c r="S11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W11" t="s" s="2">
+      <c r="X11" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="X11" t="s" s="2">
+      <c r="Y11" t="s" s="2">
         <v>89</v>
       </c>
-      <c r="Y11" t="s" s="2">
+      <c r="Z11" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA11" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB11" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC11" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD11" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE11" t="s" s="2">
         <v>90</v>
-      </c>
-      <c r="Z11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE11" t="s" s="2">
-        <v>91</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>38</v>
@@ -1659,7 +1656,7 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -1679,19 +1676,19 @@
         <v>37</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J12" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K12" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="K12" t="s" s="2">
+      <c r="L12" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="L12" t="s" s="2">
+      <c r="M12" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="M12" t="s" s="2">
-        <v>96</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -1741,7 +1738,7 @@
         <v>37</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>38</v>
@@ -1756,12 +1753,12 @@
         <v>68</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -1781,19 +1778,19 @@
         <v>37</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J13" t="s" s="2">
         <v>45</v>
       </c>
       <c r="K13" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="L13" t="s" s="2">
         <v>100</v>
       </c>
-      <c r="L13" t="s" s="2">
+      <c r="M13" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="M13" t="s" s="2">
-        <v>102</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -1843,7 +1840,7 @@
         <v>37</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>38</v>

</xml_diff>